<commit_message>
act plantilla cubicaje 2
</commit_message>
<xml_diff>
--- a/public/img/cubicaje/plantilla/Plantilla_cubicaje_actualizado_15082025.xlsx
+++ b/public/img/cubicaje/plantilla/Plantilla_cubicaje_actualizado_15082025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\forespama\public\img\cubicaje\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8102BC-5A28-421C-BC81-56BFD09B757A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89959A8E-4BB0-4D05-9640-A2D0928812DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7E53B437-93E4-489B-B999-F997A8209410}"/>
   </bookViews>
@@ -518,7 +518,7 @@
   <dimension ref="A1:D620"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4875,15 +4875,12 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <dataValidations count="3">
+  <sheetProtection algorithmName="SHA-512" hashValue="SpnM3dEjTN4XPZI+37Am95p9UU++p8QJ/ARkAvhn3ZsVk9kblkRQZSPHAkAIhvBu/gSNlAw7pWV3kspOPd87lQ==" saltValue="ogPLc6IoX/dw86x5cg53Gg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <dataValidations count="2">
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{105A2C15-C371-47DE-810D-D9A31233B48E}">
       <formula1>11</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error! Valor Maximo superado" error="El valor de diametro no puede ser mayor a 55. Verificar!" sqref="A5:A620 B6:B620" xr:uid="{43585815-9614-4503-9002-53318DECAD08}">
-      <formula1>55</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error! Valor Maximo superado" error="El valor de diametro no puede ser mayor a 55. Verificar!" sqref="B5" xr:uid="{DD8608C1-B44A-4744-950C-7E7BECB881F0}">
+    <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:B620" xr:uid="{76727A80-C1AA-4BB0-8239-6B4B11660A1F}">
       <formula1>60</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
act reporte factura sodimac detalle y plantilla cubicaje con persona
</commit_message>
<xml_diff>
--- a/public/img/cubicaje/plantilla/Plantilla_cubicaje_actualizado_15082025.xlsx
+++ b/public/img/cubicaje/plantilla/Plantilla_cubicaje_actualizado_15082025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\forespama\public\img\cubicaje\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89959A8E-4BB0-4D05-9640-A2D0928812DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758632DD-35F5-4467-95F6-0C31AE941849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7E53B437-93E4-489B-B999-F997A8209410}"/>
   </bookViews>
@@ -518,7 +518,7 @@
   <dimension ref="A1:D620"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4875,10 +4875,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="SpnM3dEjTN4XPZI+37Am95p9UU++p8QJ/ARkAvhn3ZsVk9kblkRQZSPHAkAIhvBu/gSNlAw7pWV3kspOPd87lQ==" saltValue="ogPLc6IoX/dw86x5cg53Gg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="zJfMZ7KwgHOSqb9dfU+0EYr9sXbmugmoE+aOFIzroGxczCtaCCZ5oZlEsQxnA2bs1MZqR4uxsW4xnBzm0TPbfA==" saltValue="P0I1MWBh4oJRuiXfOgwvow==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{105A2C15-C371-47DE-810D-D9A31233B48E}">
-      <formula1>11</formula1>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{105A2C15-C371-47DE-810D-D9A31233B48E}">
+      <formula1>8</formula1>
+      <formula2>11</formula2>
     </dataValidation>
     <dataValidation type="whole" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:B620" xr:uid="{76727A80-C1AA-4BB0-8239-6B4B11660A1F}">
       <formula1>60</formula1>

</xml_diff>